<commit_message>
change schema and add dim product to ssis
</commit_message>
<xml_diff>
--- a/delivery_orders.xlsx
+++ b/delivery_orders.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micaelmbp/Documents/Universidade/ENG-2022/TAAD/GlobalTech_ETL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaobraganca/Desktop/ParallelsShared/GlobalTech_ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EC7BF0-BAEB-0943-A895-4B5D144F68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733B89AB-5FB8-EB45-99A2-5739F9F93583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1900" windowWidth="46080" windowHeight="25480" xr2:uid="{7F5A1386-2A36-6240-98BC-47B3315D2513}"/>
+    <workbookView xWindow="2540" yWindow="1900" windowWidth="46080" windowHeight="25480" xr2:uid="{7F5A1386-2A36-6240-98BC-47B3315D2513}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -60,16 +60,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,24 +397,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A08B8-C4FA-EB41-837A-7B278B3E88BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E7DD78-2152-864A-BED3-5934286EEC2D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,7 +463,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>